<commit_message>
📝: finish first task
</commit_message>
<xml_diff>
--- a/docs/RGR/Lab-2-Graphs.xlsx
+++ b/docs/RGR/Lab-2-Graphs.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Оптимізація" sheetId="1" r:id="rId1"/>
-    <sheet name="Без Оптимізації" sheetId="2" r:id="rId2"/>
+    <sheet name="Оптимізація Згладжено" sheetId="3" r:id="rId2"/>
+    <sheet name="Без Оптимізації" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -166,7 +167,9 @@
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:softEdge rad="0"/>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
@@ -180,7 +183,9 @@
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:softEdge rad="0"/>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:cat>
@@ -524,6 +529,472 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="uk-UA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="uk-UA"/>
+              <a:t>З апроксимацією</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="uk-UA"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Len</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:softEdge rad="0"/>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:softEdge rad="0"/>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="6"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Оптимізація Згладжено'!$A$1:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>37500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>47500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>52500</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>57500</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>62500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Оптимізація Згладжено'!$B$1:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>5.5270000000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9649999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.4500000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.8660000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.986000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.745E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9949999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9919999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9880000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.9480000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9949999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.5230000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.99E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.0219999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.9979999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.9899999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.0119999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.9829999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.0179999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.0049999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.9789999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.0010000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.9849999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.9829999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.993E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9C5B-4226-8B89-7ABCA6BDB1E5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="943437055"/>
+        <c:axId val="943431231"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="943437055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="943431231"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="943431231"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="uk-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="943437055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="uk-UA"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="uk-UA"/>
@@ -1047,6 +1518,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1551,6 +2062,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2089,6 +3103,43 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>444499</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Діаграма 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2390,8 +3441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2631,6 +3682,250 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1">
+        <v>2500</v>
+      </c>
+      <c r="B1" s="1">
+        <v>5.5270000000000004E-4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <f>A1+A1</f>
+        <v>5000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>9.9649999999999999E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <f>A2+A1</f>
+        <v>7500</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5.4500000000000002E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <f>A3+A1</f>
+        <v>10000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9.8660000000000002E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <f>A4+A1</f>
+        <v>12500</v>
+      </c>
+      <c r="B5" s="1">
+        <v>9.986000000000001E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <f>A5+A1</f>
+        <v>15000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>9.745E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <f>A6+A1</f>
+        <v>17500</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.9949999999999998E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <f>A7+A1</f>
+        <v>20000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.9919999999999998E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <f>A8+A1</f>
+        <v>22500</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.9880000000000002E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <f>A9+A1</f>
+        <v>25000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2.9480000000000001E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <f>A10+A1</f>
+        <v>27500</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.9949999999999998E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <f>A11+A1</f>
+        <v>30000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2.5230000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <f>A12+A1</f>
+        <v>32500</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2.99E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <f>A13+A1</f>
+        <v>35000</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3.0219999999999999E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <f>A14+A1</f>
+        <v>37500</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3.9979999999999998E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <f>A15+A1</f>
+        <v>40000</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3.9899999999999996E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <f>A16+A1</f>
+        <v>42500</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3.0119999999999999E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <f>A17+A1</f>
+        <v>45000</v>
+      </c>
+      <c r="B18" s="1">
+        <v>5.9829999999999996E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <f>A18+A1</f>
+        <v>47500</v>
+      </c>
+      <c r="B19" s="1">
+        <v>4.0179999999999999E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <f>A19+A1</f>
+        <v>50000</v>
+      </c>
+      <c r="B20" s="1">
+        <v>5.0049999999999999E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <f>A20+A1</f>
+        <v>52500</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3.9789999999999999E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <f>A21+A1</f>
+        <v>55000</v>
+      </c>
+      <c r="B22" s="1">
+        <v>6.0010000000000003E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <f>A22+A1</f>
+        <v>57500</v>
+      </c>
+      <c r="B23" s="1">
+        <v>4.9849999999999998E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <f>A23+A1</f>
+        <v>60000</v>
+      </c>
+      <c r="B24" s="1">
+        <v>5.9829999999999996E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <f>A24+A1</f>
+        <v>62500</v>
+      </c>
+      <c r="B25" s="1">
+        <v>4.993E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B25"/>
   <sheetViews>

</xml_diff>